<commit_message>
feat: jump instruction with true/false
</commit_message>
<xml_diff>
--- a/Source/Instruction set.xlsx
+++ b/Source/Instruction set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Dalykai\Elektronika\FPGA\VHDL-soft-core\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853F340D-3005-4E0F-868E-92E58D4BEF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CF4713-C02B-4FC8-B129-1FFF95D7030C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>PUSH constant</t>
   </si>
@@ -94,6 +95,24 @@
   </si>
   <si>
     <t>XOR</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Pushes to top of stack</t>
+  </si>
+  <si>
+    <t>Calculates top +-*&lt;&lt;&gt;&gt; next</t>
+  </si>
+  <si>
+    <t>Loads/stores from memory location in top</t>
+  </si>
+  <si>
+    <t>Pops from top of stack N amount</t>
+  </si>
+  <si>
+    <t>Jumps to location in top if next is true/false</t>
   </si>
 </sst>
 </file>
@@ -153,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -237,11 +256,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -296,6 +324,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q23"/>
+  <dimension ref="B3:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,19 +619,11 @@
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.88671875" customWidth="1"/>
     <col min="11" max="11" width="17.77734375" customWidth="1"/>
+    <col min="12" max="12" width="39.44140625" customWidth="1"/>
     <col min="14" max="14" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -629,22 +652,10 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="3">
-        <v>3</v>
-      </c>
-      <c r="N3" s="3">
-        <v>2</v>
-      </c>
-      <c r="O3" s="3">
-        <v>1</v>
-      </c>
-      <c r="P3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C4" s="2">
         <v>1</v>
       </c>
@@ -660,23 +671,11 @@
       <c r="K4" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="4">
-        <v>0</v>
-      </c>
-      <c r="P4" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C5" s="2">
         <v>0</v>
       </c>
@@ -698,23 +697,11 @@
       <c r="K5" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0</v>
-      </c>
-      <c r="O5" s="4">
-        <v>0</v>
-      </c>
-      <c r="P5" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C6" s="2">
         <v>0</v>
       </c>
@@ -734,23 +721,11 @@
       <c r="K6" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="4">
-        <v>0</v>
-      </c>
-      <c r="N6" s="4">
-        <v>0</v>
-      </c>
-      <c r="O6" s="4">
-        <v>1</v>
-      </c>
-      <c r="P6" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C7" s="2">
         <v>0</v>
       </c>
@@ -778,23 +753,11 @@
       <c r="K7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="4">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4">
-        <v>0</v>
-      </c>
-      <c r="O7" s="4">
-        <v>1</v>
-      </c>
-      <c r="P7" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="L7" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C8" s="2">
         <v>0</v>
       </c>
@@ -814,155 +777,254 @@
       <c r="K8" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="4">
-        <v>0</v>
-      </c>
-      <c r="N8" s="4">
-        <v>1</v>
-      </c>
-      <c r="O8" s="4">
-        <v>0</v>
-      </c>
-      <c r="P8" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="L8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M9" s="4">
-        <v>0</v>
-      </c>
-      <c r="N9" s="4">
-        <v>1</v>
-      </c>
-      <c r="O9" s="4">
-        <v>0</v>
-      </c>
-      <c r="P9" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M10" s="4">
-        <v>0</v>
-      </c>
-      <c r="N10" s="4">
-        <v>1</v>
-      </c>
-      <c r="O10" s="4">
-        <v>1</v>
-      </c>
-      <c r="P10" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="s">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M11" s="4">
-        <v>0</v>
-      </c>
-      <c r="N11" s="4">
-        <v>1</v>
-      </c>
-      <c r="O11" s="4">
-        <v>1</v>
-      </c>
-      <c r="P11" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="s">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M12" s="4">
-        <v>1</v>
-      </c>
-      <c r="N12" s="4">
-        <v>0</v>
-      </c>
-      <c r="O12" s="10">
-        <v>0</v>
-      </c>
-      <c r="P12" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="s">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0</v>
+      </c>
+      <c r="G23" s="10">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="N15" s="1" t="s">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="O16" t="s">
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
         <v>16</v>
       </c>
-      <c r="P16" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="P17" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q17" t="s">
+      <c r="G27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G28" s="8">
+        <v>0</v>
+      </c>
+      <c r="H28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="P18" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q18" t="s">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G29" s="8">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N20" s="1" t="s">
+    <row r="31" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="E31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-    </row>
-    <row r="21" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="O21" t="s">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
         <v>16</v>
       </c>
-      <c r="P21" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="P22" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="P23" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q23" t="b">
+      <c r="G32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G33" s="8">
+        <v>0</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G34" s="8">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="D13:H13"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="G5:J5"/>

</xml_diff>

<commit_message>
feat: assembler auto loading big values
</commit_message>
<xml_diff>
--- a/Source/Instruction set.xlsx
+++ b/Source/Instruction set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Dalykai\Elektronika\FPGA\VHDL-soft-core\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760586D1-94D1-40F7-88F8-D8BDCE8A57FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53B9CF2-40D8-4E51-A565-14B471400146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>PUSH constant</t>
   </si>
@@ -265,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -313,9 +313,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -606,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,12 +681,14 @@
       <c r="F5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="19"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18"/>
       <c r="K5" t="s">
         <v>9</v>
       </c>
@@ -795,11 +794,8 @@
       <c r="H13" s="12"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>15</v>
-      </c>
-      <c r="D14" s="3">
-        <v>3</v>
       </c>
       <c r="E14" s="3">
         <v>2</v>
@@ -812,9 +808,6 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
       <c r="E15" s="4">
         <v>0</v>
       </c>
@@ -829,9 +822,6 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
       <c r="E16" s="4">
         <v>0</v>
       </c>
@@ -845,10 +835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D17" s="4">
-        <v>0</v>
-      </c>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E17" s="4">
         <v>0</v>
       </c>
@@ -862,10 +849,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E18" s="4">
         <v>0</v>
       </c>
@@ -879,10 +863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E19" s="4">
         <v>1</v>
       </c>
@@ -896,10 +877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E20" s="4">
         <v>1</v>
       </c>
@@ -913,10 +891,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D21" s="4">
-        <v>0</v>
-      </c>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E21" s="4">
         <v>1</v>
       </c>
@@ -930,10 +905,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D22" s="4">
-        <v>0</v>
-      </c>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E22" s="4">
         <v>1</v>
       </c>
@@ -947,10 +919,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
+    <row r="23" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E23" s="4">
         <v>0</v>
       </c>
@@ -961,14 +930,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:8" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
         <v>15</v>
       </c>
@@ -976,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:8" x14ac:dyDescent="0.3">
       <c r="G28" s="8">
         <v>0</v>
       </c>
@@ -984,7 +953,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:8" x14ac:dyDescent="0.3">
       <c r="G29" s="8">
         <v>1</v>
       </c>
@@ -992,14 +961,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E31" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:8" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +997,7 @@
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="F6:J6"/>
-    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: assembler load signed values
</commit_message>
<xml_diff>
--- a/Source/Instruction set.xlsx
+++ b/Source/Instruction set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Dalykai\Elektronika\FPGA\VHDL-soft-core\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53B9CF2-40D8-4E51-A565-14B471400146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A807D1C-8459-4005-A88B-B07AFBC1426A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>PUSH constant</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Loads/stores(next)  from/to memory location in top</t>
+  </si>
+  <si>
+    <t>Sign</t>
+  </si>
+  <si>
+    <t>Unsigned</t>
+  </si>
+  <si>
+    <t>Signed</t>
   </si>
 </sst>
 </file>
@@ -124,7 +133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +176,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -265,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -319,6 +334,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -603,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,8 +696,8 @@
       <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
+      <c r="F5" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>10</v>
@@ -835,7 +853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E17" s="4">
         <v>0</v>
       </c>
@@ -849,7 +867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E18" s="4">
         <v>0</v>
       </c>
@@ -863,7 +881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E19" s="4">
         <v>1</v>
       </c>
@@ -877,7 +895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E20" s="4">
         <v>1</v>
       </c>
@@ -891,7 +909,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E21" s="4">
         <v>1</v>
       </c>
@@ -905,7 +923,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E22" s="4">
         <v>1</v>
       </c>
@@ -919,7 +937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E23" s="4">
         <v>0</v>
       </c>
@@ -930,45 +948,66 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="I26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
         <v>15</v>
       </c>
       <c r="G27" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="J27" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.3">
       <c r="G28" s="8">
         <v>0</v>
       </c>
       <c r="H28" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="K28" s="8">
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.3">
       <c r="G29" s="8">
         <v>1</v>
       </c>
       <c r="H29" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="K29" s="8">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E31" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:12" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
         <v>15</v>
       </c>

</xml_diff>